<commit_message>
updated Learning Rate for Gradient Boosting
</commit_message>
<xml_diff>
--- a/Performance_Testing/Training-Test-Case.xlsx
+++ b/Performance_Testing/Training-Test-Case.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\GitHub\AI-Build-Carbon-Predictor\Performance_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0943601D-A721-48ED-9D44-1FBB880783B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157D4B6B-DA56-453F-9B9C-5C2B898786E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="68">
   <si>
     <t>Gradient Boosting -Test Cases</t>
   </si>
@@ -367,18 +367,6 @@
     <t>Time taken (t) / s</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Peformance (1/t)</t>
   </si>
   <si>
@@ -698,7 +686,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -714,7 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,7 +723,37 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="103">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -892,24 +909,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -917,12 +916,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -954,7 +947,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1377,7 +1376,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-935E-4900-A876-E52007F9E9BB}"/>
                   </c:ext>
@@ -1966,7 +1965,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-5110-413F-9141-7B15427F7DE2}"/>
                   </c:ext>
@@ -2208,6 +2207,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="296601791"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2523,7 +2523,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-D8DE-4095-8B27-DE388BA5C32F}"/>
                   </c:ext>
@@ -3048,7 +3048,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-66F3-4178-82FF-981F264E9EF2}"/>
                   </c:ext>
@@ -3290,6 +3290,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="212932655"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5580,7 +5581,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>790575</xdr:colOff>
+          <xdr:colOff>800100</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5666,7 +5667,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>790575</xdr:colOff>
+          <xdr:colOff>800100</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
@@ -5923,8 +5924,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>299416</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5977,8 +5978,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>361947</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6044,7 +6045,7 @@
         <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81F8438F-473F-47EE-A009-1AA18F3410EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6097,7 +6098,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BA33060-AA61-40CE-9692-9EA1C1D86802}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6150,7 +6151,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACB7143-08D3-49B9-AEFB-1186768A7DDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6203,7 +6204,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C97F2D1-6A15-4CF6-B7B2-08DFC97F28E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6256,7 +6257,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD2C6510-39C4-4871-8C98-2EA3367D4CC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6309,7 +6310,7 @@
         <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{176A4CA6-A592-4F86-87A1-3597060F7093}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6362,7 +6363,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A82D86-6C96-4AA2-BA73-CA13A531716F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6415,7 +6416,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACE8AE1-5471-4A1C-82BB-A8E1B9646575}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6468,7 +6469,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC1224F-D758-4FEB-B509-F53D330D53AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6521,7 +6522,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E401FB70-44C2-4950-A5DC-03A338229445}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6574,7 +6575,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAE59EA-551A-476A-878A-08F0ED987E8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6627,7 +6628,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA70F366-71ED-4FB4-9DBA-51DE369DF310}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6680,7 +6681,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C32B3662-8C72-4E32-A99F-E1287B500955}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6733,7 +6734,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C8F06F-DA72-4026-B5A2-FBAAFCC2FF66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6786,7 +6787,7 @@
         <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C8524A2-E6B8-4152-B0C5-A551FC9C2E36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6839,7 +6840,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B75E0539-2109-4E11-B296-13018ADD80F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6892,7 +6893,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2F0AE8-1382-4F32-9D1F-B6602A4F5FE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6945,7 +6946,7 @@
         <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AAF76CE-DD39-49D9-A19E-501FD3F3458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6998,7 +6999,7 @@
         <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4090D4-955F-49C3-963D-B2CCEF803539}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7051,7 +7052,7 @@
         <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1286C5DD-99CA-4439-A6B1-3DB4480B54A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7104,7 +7105,7 @@
         <xdr:cNvPr id="30" name="Chart 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A6ECF16-1B6B-4469-AF92-5ED4F1078CA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7142,7 +7143,7 @@
         <xdr:cNvPr id="31" name="Chart 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD84D1A-4F54-471D-265C-7FE25810D884}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7178,7 +7179,7 @@
         <xdr:cNvPr id="32" name="Chart 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62BBA71B-F385-78DC-D029-E8AF4876DBC7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7214,7 +7215,7 @@
         <xdr:cNvPr id="34" name="Chart 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C6397F-C289-E916-EFAD-6BC4908B378F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7250,7 +7251,7 @@
         <xdr:cNvPr id="35" name="Rectangle 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0183FA-E6C3-71B6-C31F-F8DCDAE32B7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7568,7 +7569,7 @@
         <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F217033-5473-4ADC-BCC7-BC934C5BA71D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7621,7 +7622,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8604C1-5171-4090-AC03-5FDCFA4C193A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7674,7 +7675,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33410B04-EA6D-477B-8B8D-876972097C87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7727,7 +7728,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10D61B21-E970-4ED0-8345-C1130929EA79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7780,7 +7781,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7999CAFE-71D7-401D-B114-6A04774001DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7833,7 +7834,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{448C254E-7737-434C-A6D8-BA46E2AD0761}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7886,7 +7887,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5FB5D50-3A86-4AFF-B8FC-52141F7E3BAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7939,7 +7940,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1FE117-1F2E-4848-AAF6-755F65E9F74D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7992,7 +7993,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B384B07-5933-497E-A8DE-3240A5C660BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8045,7 +8046,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF9204F5-B67F-44DF-A646-053075971048}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8098,7 +8099,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FDA9DB3-340D-4780-A806-A07F801585C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8151,7 +8152,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{429DFB0C-FECA-4611-B016-38EECF48D6A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8204,7 +8205,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B2D955-A611-4CB5-BF36-CD5CC1DA2624}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8257,7 +8258,7 @@
         <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9896224-E5E0-4A9A-8BF2-735FC50D535F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8310,7 +8311,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA09716-D293-4E20-BFC7-B446499D291C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8363,7 +8364,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A976613D-2AFC-4C9F-8797-F392428BE721}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8416,7 +8417,7 @@
         <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D73395-0E4F-4EAC-AD74-BA821C0151ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8469,7 +8470,7 @@
         <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C29EF13-9603-4CE4-95F6-B9EDB0826D36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8522,7 +8523,7 @@
         <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE1340D-0BC0-4399-8068-37C99F2BE1B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8575,7 +8576,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{516CE426-6BAD-460F-84B8-2CF99388F176}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8628,7 +8629,7 @@
         <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F23439A7-1F42-4D93-9481-EFB192DC8E0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8681,7 +8682,7 @@
         <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEE91B6-711B-411B-874F-5437B5A2247D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8690,6 +8691,112 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="18119912" y="2271346"/>
+          <a:ext cx="612444" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18119912" y="3795346"/>
+          <a:ext cx="612444" cy="852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18119912" y="5319346"/>
           <a:ext cx="612444" cy="852"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8730,10 +8837,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{59172835-8CA5-4901-BCA2-895A1DA6BEB5}" name="Table61416" displayName="Table61416" ref="L3:L9" totalsRowShown="0" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{59172835-8CA5-4901-BCA2-895A1DA6BEB5}" name="Table61416" displayName="Table61416" ref="L3:L9" totalsRowShown="0" dataDxfId="93">
   <autoFilter ref="L3:L9" xr:uid="{59172835-8CA5-4901-BCA2-895A1DA6BEB5}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A4840CD7-E54F-41C8-956A-FC230548500C}" name="Test case 3.0" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{A4840CD7-E54F-41C8-956A-FC230548500C}" name="Test case 3.0" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8750,10 +8857,10 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4E470563-6736-406F-860D-8CB7784EECEE}" name="Table6141618" displayName="Table6141618" ref="Q3:Q9" totalsRowShown="0" dataDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4E470563-6736-406F-860D-8CB7784EECEE}" name="Table6141618" displayName="Table6141618" ref="Q3:Q9" totalsRowShown="0" dataDxfId="91">
   <autoFilter ref="Q3:Q9" xr:uid="{4E470563-6736-406F-860D-8CB7784EECEE}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D5D452C4-B2C4-40C2-AE19-2BA5290F26E4}" name="Test case 4" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{D5D452C4-B2C4-40C2-AE19-2BA5290F26E4}" name="Test case 4" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8770,10 +8877,10 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{98AF42E9-62BE-466F-83C8-B1B63A6244B0}" name="Table622" displayName="Table622" ref="B3:B9" totalsRowShown="0" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{98AF42E9-62BE-466F-83C8-B1B63A6244B0}" name="Table622" displayName="Table622" ref="B3:B9" totalsRowShown="0" dataDxfId="89">
   <autoFilter ref="B3:B9" xr:uid="{98AF42E9-62BE-466F-83C8-B1B63A6244B0}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B298CB57-5EC8-48CE-B950-F0CDAAA4F9EB}" name="Test case 1.0" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{B298CB57-5EC8-48CE-B950-F0CDAAA4F9EB}" name="Test case 1.0" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8790,10 +8897,10 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{10719095-D610-47C3-8A41-446DB8893B3A}" name="Table62224" displayName="Table62224" ref="B19:B25" totalsRowShown="0" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{10719095-D610-47C3-8A41-446DB8893B3A}" name="Table62224" displayName="Table62224" ref="B19:B25" totalsRowShown="0" dataDxfId="87">
   <autoFilter ref="B19:B25" xr:uid="{10719095-D610-47C3-8A41-446DB8893B3A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B9966BB1-85DB-4DB7-B999-64E4F4DAFB90}" name="Test case 1.2" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{B9966BB1-85DB-4DB7-B999-64E4F4DAFB90}" name="Test case 1.2" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8810,10 +8917,10 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{50122B12-85F4-4EC7-B5E8-10829C4D9F79}" name="Table6222426" displayName="Table6222426" ref="B27:B33" totalsRowShown="0" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{50122B12-85F4-4EC7-B5E8-10829C4D9F79}" name="Table6222426" displayName="Table6222426" ref="B27:B33" totalsRowShown="0" dataDxfId="85">
   <autoFilter ref="B27:B33" xr:uid="{50122B12-85F4-4EC7-B5E8-10829C4D9F79}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D93A5190-9A98-42FC-BF4D-9B47C699CB1C}" name="Test case 1.3" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{D93A5190-9A98-42FC-BF4D-9B47C699CB1C}" name="Test case 1.3" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8830,20 +8937,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E327CB61-68E5-4C1B-82FD-B18579656A0C}" name="Table2" displayName="Table2" ref="B10:B11" totalsRowShown="0" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E327CB61-68E5-4C1B-82FD-B18579656A0C}" name="Table2" displayName="Table2" ref="B10:B11" totalsRowShown="0" dataDxfId="102">
   <autoFilter ref="B10:B11" xr:uid="{E327CB61-68E5-4C1B-82FD-B18579656A0C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{989D1204-D4AE-48BA-B9AD-6F69869EA689}" name="2.Number of Trees" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{989D1204-D4AE-48BA-B9AD-6F69869EA689}" name="2.Number of Trees" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{BE54F072-3CD2-4D02-B838-4FCFD5371453}" name="Table622242628" displayName="Table622242628" ref="B35:B41" totalsRowShown="0" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{BE54F072-3CD2-4D02-B838-4FCFD5371453}" name="Table622242628" displayName="Table622242628" ref="B35:B41" totalsRowShown="0" dataDxfId="83">
   <autoFilter ref="B35:B41" xr:uid="{BE54F072-3CD2-4D02-B838-4FCFD5371453}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BF44ED8D-8134-427C-8441-3AFF6A4CF027}" name="Test case 1.4" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{BF44ED8D-8134-427C-8441-3AFF6A4CF027}" name="Test case 1.4" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8870,10 +8977,10 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{20377698-5392-4C97-BFE3-63AF5396D1AD}" name="Table61432" displayName="Table61432" ref="G19:G25" totalsRowShown="0" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{20377698-5392-4C97-BFE3-63AF5396D1AD}" name="Table61432" displayName="Table61432" ref="G19:G25" totalsRowShown="0" dataDxfId="81">
   <autoFilter ref="G19:G25" xr:uid="{20377698-5392-4C97-BFE3-63AF5396D1AD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{09892055-1EE9-410A-9721-2362B8D8A1CE}" name="Test case 2.2" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{09892055-1EE9-410A-9721-2362B8D8A1CE}" name="Test case 2.2" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8890,10 +8997,10 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{40D3C093-0657-4302-B539-11D05DBE67AD}" name="Table61434" displayName="Table61434" ref="G27:G33" totalsRowShown="0" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{40D3C093-0657-4302-B539-11D05DBE67AD}" name="Table61434" displayName="Table61434" ref="G27:G33" totalsRowShown="0" dataDxfId="79">
   <autoFilter ref="G27:G33" xr:uid="{40D3C093-0657-4302-B539-11D05DBE67AD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{51B6FFB9-013A-4D4F-AA50-BA9A286762D1}" name="Test case 2.3" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{51B6FFB9-013A-4D4F-AA50-BA9A286762D1}" name="Test case 2.3" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8910,20 +9017,20 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{680099D7-D332-433D-A1A7-A64695907CED}" name="Table61430" displayName="Table61430" ref="G3:G9" totalsRowShown="0" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{680099D7-D332-433D-A1A7-A64695907CED}" name="Table61430" displayName="Table61430" ref="G3:G9" totalsRowShown="0" dataDxfId="77">
   <autoFilter ref="G3:G9" xr:uid="{680099D7-D332-433D-A1A7-A64695907CED}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3EB26894-844E-44B5-8E71-8F7FF61CAEC8}" name="Test case 2.0" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{3EB26894-844E-44B5-8E71-8F7FF61CAEC8}" name="Test case 2.0" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{79014818-0325-4046-9F7C-642637F8360C}" name="Table6143438" displayName="Table6143438" ref="G35:G41" totalsRowShown="0" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{79014818-0325-4046-9F7C-642637F8360C}" name="Table6143438" displayName="Table6143438" ref="G35:G41" totalsRowShown="0" dataDxfId="75">
   <autoFilter ref="G35:G41" xr:uid="{79014818-0325-4046-9F7C-642637F8360C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F995F16A-CC04-4EA8-8937-47B17DF0BF44}" name="Test case 2.4" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{F995F16A-CC04-4EA8-8937-47B17DF0BF44}" name="Test case 2.4" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8940,20 +9047,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8DF51A6-6F52-4D29-B24C-D0212FF356ED}" name="Table3" displayName="Table3" ref="B13:B15" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8DF51A6-6F52-4D29-B24C-D0212FF356ED}" name="Table3" displayName="Table3" ref="B13:B15" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <autoFilter ref="B13:B15" xr:uid="{C8DF51A6-6F52-4D29-B24C-D0212FF356ED}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DD177A92-8A2C-4B93-B911-D19418AA5516}" name="3.Learning Rate" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{DD177A92-8A2C-4B93-B911-D19418AA5516}" name="3.Learning Rate" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{55DEA20F-72BF-4B73-9A99-48BDFDE4FE8E}" name="Table614168" displayName="Table614168" ref="L11:L17" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{55DEA20F-72BF-4B73-9A99-48BDFDE4FE8E}" name="Table614168" displayName="Table614168" ref="L11:L17" totalsRowShown="0" dataDxfId="73">
   <autoFilter ref="L11:L17" xr:uid="{55DEA20F-72BF-4B73-9A99-48BDFDE4FE8E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E5C590EC-CFAB-4894-958A-CF81F5A595A8}" name="Test case 3.1" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{E5C590EC-CFAB-4894-958A-CF81F5A595A8}" name="Test case 3.1" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8970,10 +9077,10 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{987AB45D-66F1-4823-B7E2-EA687FCEEAC8}" name="Table6141610" displayName="Table6141610" ref="L19:L25" totalsRowShown="0" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{987AB45D-66F1-4823-B7E2-EA687FCEEAC8}" name="Table6141610" displayName="Table6141610" ref="L19:L25" totalsRowShown="0" dataDxfId="71">
   <autoFilter ref="L19:L25" xr:uid="{987AB45D-66F1-4823-B7E2-EA687FCEEAC8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C2525101-CC1D-498A-950B-DBBFF3636C87}" name="Test case 3" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{C2525101-CC1D-498A-950B-DBBFF3636C87}" name="Test case 3" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8990,10 +9097,10 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6BBE6077-710F-4DD5-9EDC-6491BD8003FF}" name="Table6141612" displayName="Table6141612" ref="L27:L33" totalsRowShown="0" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6BBE6077-710F-4DD5-9EDC-6491BD8003FF}" name="Table6141612" displayName="Table6141612" ref="L27:L33" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="L27:L33" xr:uid="{6BBE6077-710F-4DD5-9EDC-6491BD8003FF}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B6301974-3F61-4DB2-AF4C-B87CF4E47A5E}" name="Test case 3" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{B6301974-3F61-4DB2-AF4C-B87CF4E47A5E}" name="Test case 3" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9010,10 +9117,10 @@
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{085950E5-1974-41C0-8943-D06EF0AEF528}" name="Table6141621" displayName="Table6141621" ref="L35:L41" totalsRowShown="0" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{085950E5-1974-41C0-8943-D06EF0AEF528}" name="Table6141621" displayName="Table6141621" ref="L35:L41" totalsRowShown="0" dataDxfId="67">
   <autoFilter ref="L35:L41" xr:uid="{085950E5-1974-41C0-8943-D06EF0AEF528}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1FCE26AC-44FF-4048-BE8E-C1382781799F}" name="Test case 3" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{1FCE26AC-44FF-4048-BE8E-C1382781799F}" name="Test case 3" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9030,10 +9137,10 @@
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{5F923A8D-C6B2-4616-9211-56FFBA410F58}" name="Table614161837" displayName="Table614161837" ref="Q11:Q17" totalsRowShown="0" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{5F923A8D-C6B2-4616-9211-56FFBA410F58}" name="Table614161837" displayName="Table614161837" ref="Q11:Q17" totalsRowShown="0" dataDxfId="65">
   <autoFilter ref="Q11:Q17" xr:uid="{5F923A8D-C6B2-4616-9211-56FFBA410F58}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6625D0E8-B4B0-4574-9F49-A48D4A25C55E}" name="Test case 4" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{6625D0E8-B4B0-4574-9F49-A48D4A25C55E}" name="Test case 4" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9060,10 +9167,10 @@
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{2B6EE3E9-3472-494B-AECF-6E02C62450B9}" name="Table614161841" displayName="Table614161841" ref="Q19:Q25" totalsRowShown="0" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{2B6EE3E9-3472-494B-AECF-6E02C62450B9}" name="Table614161841" displayName="Table614161841" ref="Q19:Q25" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="Q19:Q25" xr:uid="{2B6EE3E9-3472-494B-AECF-6E02C62450B9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D925425E-A137-4BCB-88C6-AC187BAA9628}" name="Test case 4" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{D925425E-A137-4BCB-88C6-AC187BAA9628}" name="Test case 4" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9080,10 +9187,10 @@
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{989941D6-7F19-4B14-9618-EEB90DDDFCD6}" name="Table614161843" displayName="Table614161843" ref="Q27:Q33" totalsRowShown="0" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{989941D6-7F19-4B14-9618-EEB90DDDFCD6}" name="Table614161843" displayName="Table614161843" ref="Q27:Q33" totalsRowShown="0" dataDxfId="61">
   <autoFilter ref="Q27:Q33" xr:uid="{989941D6-7F19-4B14-9618-EEB90DDDFCD6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{40F1C129-337B-403F-9692-B2641BA3F3D4}" name="Test case 4" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{40F1C129-337B-403F-9692-B2641BA3F3D4}" name="Test case 4" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9100,10 +9207,10 @@
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{245A6614-8922-4938-9745-86E1A35EB9AE}" name="Table614161845" displayName="Table614161845" ref="Q35:Q41" totalsRowShown="0" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{245A6614-8922-4938-9745-86E1A35EB9AE}" name="Table614161845" displayName="Table614161845" ref="Q35:Q41" totalsRowShown="0" dataDxfId="59">
   <autoFilter ref="Q35:Q41" xr:uid="{245A6614-8922-4938-9745-86E1A35EB9AE}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C8123F23-32E3-418F-A677-3216C4C4EFC4}" name="Test case 4" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{C8123F23-32E3-418F-A677-3216C4C4EFC4}" name="Test case 4" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9123,10 +9230,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{5B4F8565-3976-454F-BB48-C6185E6358CF}" name="Table46" displayName="Table46" ref="V3:Y8" totalsRowShown="0">
   <autoFilter ref="V3:Y8" xr:uid="{5B4F8565-3976-454F-BB48-C6185E6358CF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{06AA368C-CC0F-49E1-B5BE-28D83DDB9A66}" name="Test Case" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{06AA368C-CC0F-49E1-B5BE-28D83DDB9A66}" name="Test Case" dataDxfId="57"/>
     <tableColumn id="2" xr3:uid="{41E0CB00-68CD-48B6-973E-93577CFD57FF}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{536333C5-2807-474D-80DD-A85FBD8E7D8B}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{EB33F860-94EF-432B-9B2C-B14A173CB583}" name="Performance (1/t)" dataDxfId="49">
+    <tableColumn id="5" xr3:uid="{EB33F860-94EF-432B-9B2C-B14A173CB583}" name="Performance (1/t)" dataDxfId="56">
       <calculatedColumnFormula>ROUND(1/2.3,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9138,10 +9245,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{48DC5F12-A847-492F-9F68-02D8B7442C7E}" name="Table4648" displayName="Table4648" ref="AA3:AD8" totalsRowShown="0">
   <autoFilter ref="AA3:AD8" xr:uid="{48DC5F12-A847-492F-9F68-02D8B7442C7E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{78A72A06-816E-4545-9C5C-DF931B744C42}" name="Test Case" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{78A72A06-816E-4545-9C5C-DF931B744C42}" name="Test Case" dataDxfId="55"/>
     <tableColumn id="2" xr3:uid="{9587ED8E-48F0-459F-9C8B-1CD7EF76FD70}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{F15AC4F8-9C71-48DD-82A9-87ADC7CDF894}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{BE57A6C3-7B6B-4A6F-9366-ACF5AE57B98A}" name="Peformance (1/t)" dataDxfId="47">
+    <tableColumn id="5" xr3:uid="{BE57A6C3-7B6B-4A6F-9366-ACF5AE57B98A}" name="Peformance (1/t)" dataDxfId="54">
       <calculatedColumnFormula>ROUND(1/2,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9153,10 +9260,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{3182A866-B3CD-4602-88DA-F13A7CC8EFC9}" name="Table4649" displayName="Table4649" ref="V27:Y32" totalsRowShown="0">
   <autoFilter ref="V27:Y32" xr:uid="{3182A866-B3CD-4602-88DA-F13A7CC8EFC9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7D23BEE-FD3B-4144-BF52-E38B899F7FB8}" name="Test Case" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{DCCE3EC2-A319-4931-A83E-BF1E764DF068}" name="Accuracy (%) " dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{A7D23BEE-FD3B-4144-BF52-E38B899F7FB8}" name="Test Case" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{DCCE3EC2-A319-4931-A83E-BF1E764DF068}" name="Accuracy (%) " dataDxfId="52"/>
     <tableColumn id="3" xr3:uid="{6836E4CD-871F-4FFC-8F10-1E60B2479B10}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{1B4CB6DD-5619-4C18-A548-AE1FFB7DCC46}" name="Performance (1/t)" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{1B4CB6DD-5619-4C18-A548-AE1FFB7DCC46}" name="Performance (1/t)" dataDxfId="51">
       <calculatedColumnFormula>ROUND(1/2,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9168,10 +9275,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{F5B4374B-3535-4289-872F-9069542B6AFC}" name="Table4650" displayName="Table4650" ref="AA27:AD32" totalsRowShown="0">
   <autoFilter ref="AA27:AD32" xr:uid="{F5B4374B-3535-4289-872F-9069542B6AFC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CD4DDB54-4E2B-41DB-A5C5-9DC6EF0722AF}" name="Test Case" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{CD4DDB54-4E2B-41DB-A5C5-9DC6EF0722AF}" name="Test Case" dataDxfId="50"/>
     <tableColumn id="2" xr3:uid="{EF025C8B-764D-4555-BAF2-823EEFC246AD}" name="Accuracy (%)"/>
     <tableColumn id="3" xr3:uid="{DB4DEA4E-01D9-4FC7-B119-1CAF8C027F31}" name="Time taken (t) / s"/>
-    <tableColumn id="5" xr3:uid="{8EA75FB0-D2E6-4B23-AAB1-A38114011A03}" name="Peformance (1/t)" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{8EA75FB0-D2E6-4B23-AAB1-A38114011A03}" name="Peformance (1/t)" dataDxfId="49">
       <calculatedColumnFormula>ROUND(1/8.8,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9190,10 +9297,10 @@
 </file>
 
 <file path=xl/tables/table50.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{C213463B-62B4-44BA-9DAA-F67B783BB511}" name="Table651" displayName="Table651" ref="B10:B16" totalsRowShown="0" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{C213463B-62B4-44BA-9DAA-F67B783BB511}" name="Table651" displayName="Table651" ref="B10:B16" totalsRowShown="0" dataDxfId="48">
   <autoFilter ref="B10:B16" xr:uid="{C213463B-62B4-44BA-9DAA-F67B783BB511}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{93FC11BE-D18E-401F-A733-3503F28FA0CB}" name="Test case 1.1" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{93FC11BE-D18E-401F-A733-3503F28FA0CB}" name="Test case 1.1" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9210,10 +9317,10 @@
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{A61322D7-8C4B-4823-971A-40379AE6B81D}" name="Table62253" displayName="Table62253" ref="B2:B8" totalsRowShown="0" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{A61322D7-8C4B-4823-971A-40379AE6B81D}" name="Table62253" displayName="Table62253" ref="B2:B8" totalsRowShown="0" dataDxfId="46">
   <autoFilter ref="B2:B8" xr:uid="{A61322D7-8C4B-4823-971A-40379AE6B81D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30E08E97-4A5B-4669-80EE-388EDE46E8C6}" name="Test case 1.0" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{30E08E97-4A5B-4669-80EE-388EDE46E8C6}" name="Test case 1.0" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9230,10 +9337,10 @@
 </file>
 
 <file path=xl/tables/table54.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{9F4F53F7-84DF-409F-B24A-45DC4CAB8F38}" name="Table6222455" displayName="Table6222455" ref="B18:B24" totalsRowShown="0" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{9F4F53F7-84DF-409F-B24A-45DC4CAB8F38}" name="Table6222455" displayName="Table6222455" ref="B18:B24" totalsRowShown="0" dataDxfId="44">
   <autoFilter ref="B18:B24" xr:uid="{9F4F53F7-84DF-409F-B24A-45DC4CAB8F38}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BC480597-DB85-4B0B-8399-4EA4833A4899}" name="Test case 1.2" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{BC480597-DB85-4B0B-8399-4EA4833A4899}" name="Test case 1.2" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9250,10 +9357,10 @@
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{01F09EF6-5837-4155-9EC8-730432BB99FC}" name="Table622245557" displayName="Table622245557" ref="B26:B32" totalsRowShown="0" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{01F09EF6-5837-4155-9EC8-730432BB99FC}" name="Table622245557" displayName="Table622245557" ref="B26:B32" totalsRowShown="0" dataDxfId="42">
   <autoFilter ref="B26:B32" xr:uid="{01F09EF6-5837-4155-9EC8-730432BB99FC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2EE3C7CA-C173-407B-AAE7-264002AE23EB}" name="Test case 1.2" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{2EE3C7CA-C173-407B-AAE7-264002AE23EB}" name="Test case 1.2" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9270,10 +9377,10 @@
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{6394B0B7-D791-4076-A0E8-AE260737AF34}" name="Table622245559" displayName="Table622245559" ref="B34:B40" totalsRowShown="0" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{6394B0B7-D791-4076-A0E8-AE260737AF34}" name="Table622245559" displayName="Table622245559" ref="B34:B40" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="B34:B40" xr:uid="{6394B0B7-D791-4076-A0E8-AE260737AF34}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A74583AA-662C-452C-A02F-B47C5C76CC9E}" name="Test case 1.2" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{A74583AA-662C-452C-A02F-B47C5C76CC9E}" name="Test case 1.2" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9290,20 +9397,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D9F279F8-EA83-410B-A2A3-94F10A77AE95}" name="Table6" displayName="Table6" ref="B11:B17" totalsRowShown="0" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D9F279F8-EA83-410B-A2A3-94F10A77AE95}" name="Table6" displayName="Table6" ref="B11:B17" totalsRowShown="0" dataDxfId="97">
   <autoFilter ref="B11:B17" xr:uid="{D9F279F8-EA83-410B-A2A3-94F10A77AE95}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{887B0203-4A77-4EC9-9590-D47DD57CEE09}" name="Test case 1.1" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{887B0203-4A77-4EC9-9590-D47DD57CEE09}" name="Test case 1.1" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="62" xr:uid="{FE1FAEC8-BFCE-4CBA-952F-C7C97B40839A}" name="Table61463" displayName="Table61463" ref="G2:G8" totalsRowShown="0" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="62" xr:uid="{FE1FAEC8-BFCE-4CBA-952F-C7C97B40839A}" name="Table61463" displayName="Table61463" ref="G2:G8" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="G2:G8" xr:uid="{FE1FAEC8-BFCE-4CBA-952F-C7C97B40839A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E715A345-B4C8-4A1A-B30A-196C86199B10}" name="Test case 2.0" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{E715A345-B4C8-4A1A-B30A-196C86199B10}" name="Test case 2.0" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9320,10 +9427,10 @@
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{FE5F3815-582E-4FA9-89F0-FB72AA39C1F3}" name="Table6146365" displayName="Table6146365" ref="G10:G16" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{FE5F3815-582E-4FA9-89F0-FB72AA39C1F3}" name="Table6146365" displayName="Table6146365" ref="G10:G16" totalsRowShown="0" dataDxfId="36">
   <autoFilter ref="G10:G16" xr:uid="{FE5F3815-582E-4FA9-89F0-FB72AA39C1F3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B7208465-D331-484D-A818-ABD5CB1964DA}" name="Test case 2.1" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{B7208465-D331-484D-A818-ABD5CB1964DA}" name="Test case 2.1" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9340,10 +9447,10 @@
 </file>
 
 <file path=xl/tables/table64.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="66" xr:uid="{E007C985-170F-48A9-91E3-5B1DC841409A}" name="Table6146367" displayName="Table6146367" ref="G18:G24" totalsRowShown="0" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="66" xr:uid="{E007C985-170F-48A9-91E3-5B1DC841409A}" name="Table6146367" displayName="Table6146367" ref="G18:G24" totalsRowShown="0" dataDxfId="34">
   <autoFilter ref="G18:G24" xr:uid="{E007C985-170F-48A9-91E3-5B1DC841409A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2C45AA0E-D4E4-4890-B5C7-06281DE2CE40}" name="Test case 2.2" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{2C45AA0E-D4E4-4890-B5C7-06281DE2CE40}" name="Test case 2.2" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9360,10 +9467,10 @@
 </file>
 
 <file path=xl/tables/table66.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="68" xr:uid="{F94E8711-B090-4D1C-967F-B0C77F5830A3}" name="Table6146369" displayName="Table6146369" ref="G26:G32" totalsRowShown="0" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="68" xr:uid="{F94E8711-B090-4D1C-967F-B0C77F5830A3}" name="Table6146369" displayName="Table6146369" ref="G26:G32" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="G26:G32" xr:uid="{F94E8711-B090-4D1C-967F-B0C77F5830A3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2EABB598-EE1D-4E53-8EC8-0F6224B8EABE}" name="Test case 2.3" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{2EABB598-EE1D-4E53-8EC8-0F6224B8EABE}" name="Test case 2.3" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9380,10 +9487,10 @@
 </file>
 
 <file path=xl/tables/table68.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="70" xr:uid="{95E01781-6E98-4571-A778-1B66617D15AC}" name="Table6146371" displayName="Table6146371" ref="G34:G40" totalsRowShown="0" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="70" xr:uid="{95E01781-6E98-4571-A778-1B66617D15AC}" name="Table6146371" displayName="Table6146371" ref="G34:G40" totalsRowShown="0" dataDxfId="30">
   <autoFilter ref="G34:G40" xr:uid="{95E01781-6E98-4571-A778-1B66617D15AC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{13A0D282-BDFB-42B4-ACD2-B0220BE4D822}" name="Test case 2.4" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{13A0D282-BDFB-42B4-ACD2-B0220BE4D822}" name="Test case 2.4" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9410,10 +9517,10 @@
 </file>
 
 <file path=xl/tables/table70.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{40709BAD-7E55-40A0-AEEE-8D55E9E4BD3E}" name="Table614637173" displayName="Table614637173" ref="G42:G48" totalsRowShown="0" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{40709BAD-7E55-40A0-AEEE-8D55E9E4BD3E}" name="Table614637173" displayName="Table614637173" ref="G42:G48" totalsRowShown="0" dataDxfId="28">
   <autoFilter ref="G42:G48" xr:uid="{40709BAD-7E55-40A0-AEEE-8D55E9E4BD3E}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5ABF6B1D-FCD8-4D37-AD63-291983D6F83C}" name="Test case 2.5" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{5ABF6B1D-FCD8-4D37-AD63-291983D6F83C}" name="Test case 2.5" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9430,10 +9537,10 @@
 </file>
 
 <file path=xl/tables/table72.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{31C76E84-4F4D-4E43-B640-C49141C97BC6}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{31C76E84-4F4D-4E43-B640-C49141C97BC6}" name="Table6141675" displayName="Table6141675" ref="L2:L8" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="L2:L8" xr:uid="{31C76E84-4F4D-4E43-B640-C49141C97BC6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{BE07116B-D2DA-4E53-A11F-3EFA575405EA}" name="Test case 3.0.0" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{BE07116B-D2DA-4E53-A11F-3EFA575405EA}" name="Test case 3.0.0" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9450,10 +9557,10 @@
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{E49B1298-90A5-4673-944E-28448F5AFDC7}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{E49B1298-90A5-4673-944E-28448F5AFDC7}" name="Table614167577" displayName="Table614167577" ref="L10:L16" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="L10:L16" xr:uid="{E49B1298-90A5-4673-944E-28448F5AFDC7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0DC3EC41-41DB-439A-90BB-7E815F54AAF6}" name="Test case 3.0.1" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{0DC3EC41-41DB-439A-90BB-7E815F54AAF6}" name="Test case 3.0.1" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9464,17 +9571,17 @@
   <autoFilter ref="N10:O16" xr:uid="{8333D9DA-093A-496D-BB43-6DC79B00DB2C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2514BE37-02DB-4B79-85A8-20A73CB14AAE}" name="Results "/>
-    <tableColumn id="3" xr3:uid="{E98007C2-FDD0-4678-A32A-850C98D85787}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E98007C2-FDD0-4678-A32A-850C98D85787}" name="Column1" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table76.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{2D809994-DB62-4CF2-A543-EA36280023FB}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{2D809994-DB62-4CF2-A543-EA36280023FB}" name="Table614167579" displayName="Table614167579" ref="L18:L24" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="L18:L24" xr:uid="{2D809994-DB62-4CF2-A543-EA36280023FB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{50F9FC3B-99E7-4093-ACFD-633F3C8249CA}" name="Test case 3.0.2" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{50F9FC3B-99E7-4093-ACFD-633F3C8249CA}" name="Test case 3.0.2" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9491,10 +9598,10 @@
 </file>
 
 <file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{956F1139-7DE2-4DE3-BD69-80E3C686792D}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{956F1139-7DE2-4DE3-BD69-80E3C686792D}" name="Table614167581" displayName="Table614167581" ref="L26:L32" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="L26:L32" xr:uid="{956F1139-7DE2-4DE3-BD69-80E3C686792D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E7A6DCE6-1FCB-4C58-B076-1CF0FB68D1AE}" name="Test case 3.0.3" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{E7A6DCE6-1FCB-4C58-B076-1CF0FB68D1AE}" name="Test case 3.0.3" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9511,20 +9618,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{16D1170F-46DF-403A-BDA5-A7F369BC6A27}" name="Table614" displayName="Table614" ref="G11:G17" totalsRowShown="0" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{16D1170F-46DF-403A-BDA5-A7F369BC6A27}" name="Table614" displayName="Table614" ref="G11:G17" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="G11:G17" xr:uid="{16D1170F-46DF-403A-BDA5-A7F369BC6A27}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B18CDA0E-2455-43A8-B327-690DCD4462B1}" name="Test case 2.1" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{B18CDA0E-2455-43A8-B327-690DCD4462B1}" name="Test case 2.1" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table80.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{FBF0D207-44DD-4351-B755-1A5175A2CB03}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{FBF0D207-44DD-4351-B755-1A5175A2CB03}" name="Table614167583" displayName="Table614167583" ref="L34:L40" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="L34:L40" xr:uid="{FBF0D207-44DD-4351-B755-1A5175A2CB03}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B1BE015F-B6D6-4364-9A7B-03BC3CB262AD}" name="Test case 3.0.4" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{B1BE015F-B6D6-4364-9A7B-03BC3CB262AD}" name="Test case 3.0.4" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9541,10 +9648,10 @@
 </file>
 
 <file path=xl/tables/table82.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{A179E447-4836-4456-8237-49134D0C5AB1}" name="Table61416887" displayName="Table61416887" ref="Q2:Q8" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{A179E447-4836-4456-8237-49134D0C5AB1}" name="Table61416887" displayName="Table61416887" ref="Q2:Q8" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="Q2:Q8" xr:uid="{A179E447-4836-4456-8237-49134D0C5AB1}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3AC72BC0-4EFE-4477-A722-FCAF5DE98629}" name="Test case 3.1.0" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3AC72BC0-4EFE-4477-A722-FCAF5DE98629}" name="Test case 3.1.0" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9561,10 +9668,10 @@
 </file>
 
 <file path=xl/tables/table84.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{ED4A661A-49C2-48DA-96A7-01349958B69A}" name="Table6141688789" displayName="Table6141688789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{ED4A661A-49C2-48DA-96A7-01349958B69A}" name="Table6141688789" displayName="Table6141688789" ref="Q10:Q16" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="Q10:Q16" xr:uid="{ED4A661A-49C2-48DA-96A7-01349958B69A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C4D482EE-56D5-477C-968D-0FC234B9532F}" name="Test case 3.1.1" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{C4D482EE-56D5-477C-968D-0FC234B9532F}" name="Test case 3.1.1" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9581,10 +9688,10 @@
 </file>
 
 <file path=xl/tables/table86.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{AD56A7BE-2009-4A28-9059-C855A0B8ADDF}" name="Table614168878993" displayName="Table614168878993" ref="Q18:Q24" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="92" xr:uid="{AD56A7BE-2009-4A28-9059-C855A0B8ADDF}" name="Table614168878993" displayName="Table614168878993" ref="Q18:Q24" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="Q18:Q24" xr:uid="{AD56A7BE-2009-4A28-9059-C855A0B8ADDF}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1D209EEC-571C-45BE-8AFC-4665C274EAA9}" name="Test case 3.1.2" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{1D209EEC-571C-45BE-8AFC-4665C274EAA9}" name="Test case 3.1.2" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9601,10 +9708,10 @@
 </file>
 
 <file path=xl/tables/table88.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{69255ABD-32CD-44A2-8D21-16C1467815E2}" name="Table61416184195" displayName="Table61416184195" ref="V2:V8" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="94" xr:uid="{69255ABD-32CD-44A2-8D21-16C1467815E2}" name="Table61416184195" displayName="Table61416184195" ref="V2:V8" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="V2:V8" xr:uid="{69255ABD-32CD-44A2-8D21-16C1467815E2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{486FE4AA-332B-44D8-BE13-D1DDBE285583}" name="Test case 4" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{486FE4AA-332B-44D8-BE13-D1DDBE285583}" name="Test case 4" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9631,10 +9738,10 @@
 </file>
 
 <file path=xl/tables/table90.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{CF64DBCF-74FF-4CAE-A344-CD484EB270EA}" name="Table6141618419597" displayName="Table6141618419597" ref="V10:V16" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="96" xr:uid="{CF64DBCF-74FF-4CAE-A344-CD484EB270EA}" name="Table6141618419597" displayName="Table6141618419597" ref="V10:V16" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="V10:V16" xr:uid="{CF64DBCF-74FF-4CAE-A344-CD484EB270EA}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CEB3598B-DF87-4F29-8D63-7D942728A389}" name="Test case 4" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CEB3598B-DF87-4F29-8D63-7D942728A389}" name="Test case 4" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9651,10 +9758,10 @@
 </file>
 
 <file path=xl/tables/table92.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{8E57DA44-9CFA-4675-8450-A36A7DBFB3C5}" name="Table614161841959799" displayName="Table614161841959799" ref="V18:V24" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{8E57DA44-9CFA-4675-8450-A36A7DBFB3C5}" name="Table614161841959799" displayName="Table614161841959799" ref="V18:V24" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="V18:V24" xr:uid="{8E57DA44-9CFA-4675-8450-A36A7DBFB3C5}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FCBC0CE6-80F1-488E-B0E2-2F51EB855348}" name="Test case 4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FCBC0CE6-80F1-488E-B0E2-2F51EB855348}" name="Test case 4" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9665,6 +9772,46 @@
   <autoFilter ref="X18:X24" xr:uid="{69C0DFBB-951D-4B72-B1EE-EE7D382B0132}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{708C122C-8F7A-483D-B596-93061077A487}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table94.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{3628D8D0-624C-409C-BBA7-6A610FF516B4}" name="Table61416184195979961" displayName="Table61416184195979961" ref="V26:V32" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="V26:V32" xr:uid="{3628D8D0-624C-409C-BBA7-6A610FF516B4}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CF1A969B-5902-4A2B-90E7-0C4EDF46CF05}" name="Test case 4" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table95.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="61" xr:uid="{2F2906BC-A0CC-4C0F-9546-110F8343E07C}" name="Table1215171942969810062" displayName="Table1215171942969810062" ref="X26:X32" totalsRowShown="0">
+  <autoFilter ref="X26:X32" xr:uid="{2F2906BC-A0CC-4C0F-9546-110F8343E07C}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{884C4753-DCDA-4594-8C38-1FD61B86143D}" name="Results "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{3B8AEC20-A150-4AB2-BB93-2A9266035C55}" name="Table6141618419597996185" displayName="Table6141618419597996185" ref="V34:V40" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="V34:V40" xr:uid="{3B8AEC20-A150-4AB2-BB93-2A9266035C55}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{12ED3CDC-BBD5-4F0B-B225-FE3D63F9C015}" name="Test case 4" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table97.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="85" xr:uid="{DDBD95E2-B582-444A-8D05-F58CD9D0611B}" name="Table121517194296981006286" displayName="Table121517194296981006286" ref="X34:X40" totalsRowShown="0">
+  <autoFilter ref="X34:X40" xr:uid="{DDBD95E2-B582-444A-8D05-F58CD9D0611B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{671A55CC-8124-4AFC-AC07-7F4D0221AA19}" name="Results "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9933,15 +10080,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W4" sqref="E4:W42"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
@@ -9996,7 +10144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="22.5" customHeight="1">
+    <row r="18" spans="2:3" ht="33" customHeight="1">
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
@@ -10134,10 +10282,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8A34A8-B14D-4397-8E12-6D9029D23CEA}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AD41"/>
   <sheetViews>
-    <sheetView topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19:T25"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10196,7 +10345,7 @@
       <c r="Y3" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AA3" s="10" t="s">
         <v>45</v>
       </c>
       <c r="AB3" t="s">
@@ -10206,7 +10355,7 @@
         <v>51</v>
       </c>
       <c r="AD3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:30" ht="15.75" thickBot="1">
@@ -10234,7 +10383,7 @@
       <c r="N4" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>282439.04622646602</v>
       </c>
       <c r="Q4" s="6" t="s">
@@ -10246,7 +10395,7 @@
       <c r="T4" s="7">
         <v>12768.6901565349</v>
       </c>
-      <c r="V4" s="11">
+      <c r="V4" s="10">
         <v>1</v>
       </c>
       <c r="W4">
@@ -10259,7 +10408,7 @@
         <f>ROUND(1/2.3,2)</f>
         <v>0.43</v>
       </c>
-      <c r="AA4" s="11">
+      <c r="AA4" s="10">
         <v>2</v>
       </c>
       <c r="AB4">
@@ -10269,7 +10418,7 @@
         <v>2</v>
       </c>
       <c r="AD4">
-        <f t="shared" ref="AD4:AD8" si="0">ROUND(1/2,2)</f>
+        <f t="shared" ref="AD4" si="0">ROUND(1/2,2)</f>
         <v>0.5</v>
       </c>
     </row>
@@ -10298,7 +10447,7 @@
       <c r="N5" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>531.44994705660304</v>
       </c>
       <c r="Q5" s="6" t="s">
@@ -10310,29 +10459,29 @@
       <c r="T5" s="7">
         <v>112.99862900289899</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W5" s="14">
+      <c r="W5" s="13">
         <v>97</v>
       </c>
-      <c r="X5" s="14">
+      <c r="X5" s="13">
         <v>3.1</v>
       </c>
-      <c r="Y5" s="15">
+      <c r="Y5" s="14">
         <f>ROUND(1/3.1,2)</f>
         <v>0.32</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AA5" s="12">
         <v>2.1</v>
       </c>
-      <c r="AB5" s="14">
+      <c r="AB5" s="13">
         <v>96</v>
       </c>
-      <c r="AC5" s="14">
+      <c r="AC5" s="13">
         <v>2.5</v>
       </c>
-      <c r="AD5" s="15">
+      <c r="AD5" s="14">
         <f>ROUND(1/2.5,2)</f>
         <v>0.4</v>
       </c>
@@ -10362,7 +10511,7 @@
       <c r="N6" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="7">
         <v>268.23323563194202</v>
       </c>
       <c r="Q6" s="6" t="s">
@@ -10374,7 +10523,7 @@
       <c r="T6" s="7">
         <v>58.074218371518299</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6" s="10">
         <v>1.2</v>
       </c>
       <c r="W6">
@@ -10387,7 +10536,7 @@
         <f>ROUND(1/3.6,2)</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6" s="10">
         <v>2.2000000000000002</v>
       </c>
       <c r="AB6">
@@ -10426,7 +10575,7 @@
       <c r="N7" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="7">
         <v>0.79286796800025305</v>
       </c>
       <c r="Q7" s="6" t="s">
@@ -10438,7 +10587,7 @@
       <c r="T7" s="7">
         <v>0.50464613546282899</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="10">
         <v>1.3</v>
       </c>
       <c r="W7">
@@ -10451,7 +10600,7 @@
         <f>ROUND(1/4.3,2)</f>
         <v>0.23</v>
       </c>
-      <c r="AA7" s="11">
+      <c r="AA7" s="10">
         <v>2.2999999999999998</v>
       </c>
       <c r="AB7">
@@ -10487,10 +10636,10 @@
       <c r="L8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="N8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>-0.22424700327413699</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -10502,7 +10651,7 @@
       <c r="T8" s="7">
         <v>0.94465343631227305</v>
       </c>
-      <c r="V8" s="11">
+      <c r="V8" s="10">
         <v>1.4</v>
       </c>
       <c r="W8">
@@ -10515,7 +10664,7 @@
         <f>ROUND(1/5.1,2)</f>
         <v>0.2</v>
       </c>
-      <c r="AA8" s="11">
+      <c r="AA8" s="10">
         <v>2.4</v>
       </c>
       <c r="AB8">
@@ -10554,19 +10703,19 @@
       <c r="N9" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="7">
         <v>2</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="17">
+      <c r="T9" s="16">
         <v>8.8000000000000007</v>
       </c>
-      <c r="V9" s="11"/>
+      <c r="V9" s="10"/>
     </row>
     <row r="11" spans="2:30">
       <c r="B11" t="s">
@@ -10601,7 +10750,7 @@
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>6680.91</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -10610,7 +10759,7 @@
       <c r="I12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="17">
         <v>9557.1229944185106</v>
       </c>
       <c r="L12" s="6" t="s">
@@ -10639,7 +10788,7 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>81.736999999999995</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -10648,7 +10797,7 @@
       <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="17">
         <v>97.760539045253296</v>
       </c>
       <c r="L13" s="6" t="s">
@@ -10677,7 +10826,7 @@
       <c r="D14" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <v>39.326000000000001</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -10686,7 +10835,7 @@
       <c r="I14" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="17">
         <v>43.867895317494799</v>
       </c>
       <c r="L14" s="6" t="s">
@@ -10715,7 +10864,7 @@
       <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>0.25800000000000001</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -10724,7 +10873,7 @@
       <c r="I15" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <v>0.29403942636080099</v>
       </c>
       <c r="L15" s="6" t="s">
@@ -10753,7 +10902,7 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <v>0.97099999999999997</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -10762,16 +10911,16 @@
       <c r="I16" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="17">
         <v>0.95857414425462295</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="16" t="s">
+      <c r="N16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="16">
         <v>-0.22424703428017301</v>
       </c>
       <c r="Q16" s="6" t="s">
@@ -10791,7 +10940,7 @@
       <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="18">
         <v>3.1</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -10800,7 +10949,7 @@
       <c r="I17" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="18">
         <v>2.5</v>
       </c>
       <c r="L17" s="6" t="s">
@@ -10815,13 +10964,13 @@
       <c r="Q17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S17" s="16" t="s">
+      <c r="S17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T17" s="17">
+      <c r="T17" s="16">
         <v>15.6</v>
       </c>
-      <c r="V17" s="11"/>
+      <c r="V17" s="10"/>
     </row>
     <row r="19" spans="2:30">
       <c r="B19" t="s">
@@ -10883,7 +11032,7 @@
       <c r="S20" t="s">
         <v>20</v>
       </c>
-      <c r="T20" s="18">
+      <c r="T20" s="17">
         <v>8229.2994916500102</v>
       </c>
     </row>
@@ -10921,7 +11070,7 @@
       <c r="S21" t="s">
         <v>21</v>
       </c>
-      <c r="T21" s="18">
+      <c r="T21" s="17">
         <v>90.715486503959198</v>
       </c>
     </row>
@@ -10959,7 +11108,7 @@
       <c r="S22" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="18">
+      <c r="T22" s="17">
         <v>45.415053024014597</v>
       </c>
     </row>
@@ -10997,7 +11146,7 @@
       <c r="S23" t="s">
         <v>23</v>
       </c>
-      <c r="T23" s="18">
+      <c r="T23" s="17">
         <v>0.40764766301183403</v>
       </c>
     </row>
@@ -11023,10 +11172,10 @@
       <c r="L24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N24" s="16" t="s">
+      <c r="N24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="17">
+      <c r="O24" s="16">
         <v>-0.224247000490162</v>
       </c>
       <c r="Q24" s="6" t="s">
@@ -11035,7 +11184,7 @@
       <c r="S24" t="s">
         <v>24</v>
       </c>
-      <c r="T24" s="18">
+      <c r="T24" s="17">
         <v>0.964329665546244</v>
       </c>
     </row>
@@ -11070,13 +11219,13 @@
       <c r="Q25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S25" s="16" t="s">
+      <c r="S25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T25" s="17">
+      <c r="T25" s="16">
         <v>22</v>
       </c>
-      <c r="V25" s="11"/>
+      <c r="V25" s="10"/>
     </row>
     <row r="27" spans="2:30">
       <c r="B27" t="s">
@@ -11103,11 +11252,11 @@
       <c r="S27" t="s">
         <v>19</v>
       </c>
-      <c r="V27" s="11" t="s">
+      <c r="V27" s="10" t="s">
         <v>45</v>
       </c>
       <c r="W27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="X27" t="s">
         <v>51</v>
@@ -11115,7 +11264,7 @@
       <c r="Y27" t="s">
         <v>50</v>
       </c>
-      <c r="AA27" s="11" t="s">
+      <c r="AA27" s="10" t="s">
         <v>45</v>
       </c>
       <c r="AB27" t="s">
@@ -11125,7 +11274,7 @@
         <v>51</v>
       </c>
       <c r="AD27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:30">
@@ -11162,23 +11311,23 @@
       <c r="S28" t="s">
         <v>20</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28" s="7">
         <v>6397.8670741624801</v>
       </c>
-      <c r="V28" s="11">
+      <c r="V28" s="10">
         <v>3</v>
       </c>
-      <c r="W28" s="12">
+      <c r="W28" s="11">
         <v>-0.2</v>
       </c>
       <c r="X28">
         <v>2</v>
       </c>
       <c r="Y28">
-        <f t="shared" ref="Y28:Y32" si="1">ROUND(1/2,2)</f>
+        <f t="shared" ref="Y28" si="1">ROUND(1/2,2)</f>
         <v>0.5</v>
       </c>
-      <c r="AA28" s="11">
+      <c r="AA28" s="10">
         <v>4</v>
       </c>
       <c r="AB28">
@@ -11187,8 +11336,8 @@
       <c r="AC28">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AD28" s="10">
-        <f t="shared" ref="AD28:AD32" si="2">ROUND(1/8.8,2)</f>
+      <c r="AD28" s="9">
+        <f t="shared" ref="AD28" si="2">ROUND(1/8.8,2)</f>
         <v>0.11</v>
       </c>
     </row>
@@ -11226,13 +11375,13 @@
       <c r="S29" t="s">
         <v>21</v>
       </c>
-      <c r="T29" s="9">
+      <c r="T29" s="7">
         <v>79.986668102643705</v>
       </c>
-      <c r="V29" s="11">
+      <c r="V29" s="10">
         <v>3.1</v>
       </c>
-      <c r="W29" s="12">
+      <c r="W29" s="11">
         <v>-0.2</v>
       </c>
       <c r="X29">
@@ -11242,7 +11391,7 @@
         <f>ROUND(1/2.2,2)</f>
         <v>0.45</v>
       </c>
-      <c r="AA29" s="11">
+      <c r="AA29" s="10">
         <v>4.0999999999999996</v>
       </c>
       <c r="AB29">
@@ -11251,7 +11400,7 @@
       <c r="AC29">
         <v>15.6</v>
       </c>
-      <c r="AD29" s="10">
+      <c r="AD29" s="9">
         <f>ROUND(1/15.6,2)</f>
         <v>0.06</v>
       </c>
@@ -11290,13 +11439,13 @@
       <c r="S30" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="9">
+      <c r="T30" s="7">
         <v>39.340431837441102</v>
       </c>
-      <c r="V30" s="11">
+      <c r="V30" s="10">
         <v>3.2</v>
       </c>
-      <c r="W30" s="12">
+      <c r="W30" s="11">
         <v>-0.2</v>
       </c>
       <c r="X30">
@@ -11306,16 +11455,16 @@
         <f>ROUND(1/2.4,2)</f>
         <v>0.42</v>
       </c>
-      <c r="AA30" s="13">
+      <c r="AA30" s="12">
         <v>4.2</v>
       </c>
-      <c r="AB30" s="14">
+      <c r="AB30" s="13">
         <v>96</v>
       </c>
-      <c r="AC30" s="14">
+      <c r="AC30" s="13">
         <v>22</v>
       </c>
-      <c r="AD30" s="14">
+      <c r="AD30" s="13">
         <f>ROUND(1/22,2)</f>
         <v>0.05</v>
       </c>
@@ -11354,13 +11503,13 @@
       <c r="S31" t="s">
         <v>23</v>
       </c>
-      <c r="T31" s="9">
+      <c r="T31" s="7">
         <v>0.362879096644458</v>
       </c>
-      <c r="V31" s="11">
+      <c r="V31" s="10">
         <v>3.3</v>
       </c>
-      <c r="W31" s="12">
+      <c r="W31" s="11">
         <v>-0.2</v>
       </c>
       <c r="X31">
@@ -11370,7 +11519,7 @@
         <f>ROUND(1/2.7,2)</f>
         <v>0.37</v>
       </c>
-      <c r="AA31" s="11">
+      <c r="AA31" s="10">
         <v>4.3</v>
       </c>
       <c r="AB31">
@@ -11379,7 +11528,7 @@
       <c r="AC31">
         <v>29</v>
       </c>
-      <c r="AD31" s="10">
+      <c r="AD31" s="9">
         <f>ROUND(1/29,2)</f>
         <v>0.03</v>
       </c>
@@ -11406,10 +11555,10 @@
       <c r="L32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N32" s="16" t="s">
+      <c r="N32" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O32" s="17">
+      <c r="O32" s="16">
         <v>-0.22424690045922299</v>
       </c>
       <c r="Q32" s="6" t="s">
@@ -11418,13 +11567,13 @@
       <c r="S32" t="s">
         <v>24</v>
       </c>
-      <c r="T32" s="9">
+      <c r="T32" s="7">
         <v>0.97226810634883198</v>
       </c>
-      <c r="V32" s="11">
+      <c r="V32" s="10">
         <v>3.4</v>
       </c>
-      <c r="W32" s="12">
+      <c r="W32" s="11">
         <v>-0.2</v>
       </c>
       <c r="X32">
@@ -11434,7 +11583,7 @@
         <f>ROUND(1/2.9,2)</f>
         <v>0.34</v>
       </c>
-      <c r="AA32" s="11">
+      <c r="AA32" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AB32">
@@ -11443,7 +11592,7 @@
       <c r="AC32">
         <v>50</v>
       </c>
-      <c r="AD32" s="10">
+      <c r="AD32" s="9">
         <f>ROUND(1/50,2)</f>
         <v>0.02</v>
       </c>
@@ -11479,10 +11628,10 @@
       <c r="Q33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S33" s="16" t="s">
+      <c r="S33" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T33" s="17">
+      <c r="T33" s="16">
         <v>29</v>
       </c>
     </row>
@@ -11689,10 +11838,10 @@
       <c r="L40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N40" s="16" t="s">
+      <c r="N40" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O40" s="17">
+      <c r="O40" s="16">
         <v>-0.22424694640234899</v>
       </c>
       <c r="Q40" s="6" t="s">
@@ -11736,10 +11885,10 @@
       <c r="Q41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S41" s="16" t="s">
+      <c r="S41" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T41" s="17">
+      <c r="T41" s="16">
         <v>50</v>
       </c>
     </row>
@@ -11800,10 +11949,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5618ECCB-8A09-44EC-AB46-519C3D12A472}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11831,13 +11981,13 @@
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S2" t="s">
         <v>19</v>
@@ -11874,7 +12024,7 @@
       <c r="N3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <v>282439.04622646602</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -11921,7 +12071,7 @@
       <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>531.44994705660304</v>
       </c>
       <c r="Q4" s="6" t="s">
@@ -11968,7 +12118,7 @@
       <c r="N5" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>268.23323563194202</v>
       </c>
       <c r="Q5" s="6" t="s">
@@ -12015,7 +12165,7 @@
       <c r="N6" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="7">
         <v>0.79286796800025305</v>
       </c>
       <c r="Q6" s="6" t="s">
@@ -12059,19 +12209,19 @@
       <c r="L7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="16">
         <v>-0.22424700327413699</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="16">
         <v>-0.22424703428017301</v>
       </c>
       <c r="V7" s="6" t="s">
@@ -12109,7 +12259,7 @@
       <c r="N8" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="7">
         <v>2</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -12124,10 +12274,10 @@
       <c r="V8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="X8" s="16" t="s">
+      <c r="X8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="Y8" s="17">
+      <c r="Y8" s="16">
         <v>22</v>
       </c>
     </row>
@@ -12145,7 +12295,7 @@
         <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
         <v>19</v>
@@ -12154,7 +12304,7 @@
         <v>42</v>
       </c>
       <c r="Q10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="S10" t="s">
         <v>19</v>
@@ -12191,7 +12341,7 @@
       <c r="N11" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="7">
         <v>250374.36231508001</v>
       </c>
       <c r="Q11" s="6" t="s">
@@ -12238,7 +12388,7 @@
       <c r="N12" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="7">
         <v>500.37422227277</v>
       </c>
       <c r="Q12" s="6" t="s">
@@ -12262,7 +12412,7 @@
     </row>
     <row r="13" spans="2:25">
       <c r="B13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -12271,7 +12421,7 @@
         <v>33.264314645031199</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
@@ -12280,16 +12430,16 @@
         <v>35.1996051287651</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="N13" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="7">
         <v>244.727096954345</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="S13" t="s">
         <v>22</v>
@@ -12298,7 +12448,7 @@
         <v>244.727114253997</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="X13" t="s">
         <v>22</v>
@@ -12332,7 +12482,7 @@
       <c r="N14" t="s">
         <v>23</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="7">
         <v>0.77520813040362702</v>
       </c>
       <c r="Q14" s="6" t="s">
@@ -12376,19 +12526,19 @@
       <c r="L15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="N15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="16">
         <v>-8.5260932778872395E-2</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S15" s="16" t="s">
+      <c r="S15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T15" s="17">
+      <c r="T15" s="16">
         <v>-8.5260988769203502E-2</v>
       </c>
       <c r="V15" s="6" t="s">
@@ -12426,7 +12576,7 @@
       <c r="N16" t="s">
         <v>38</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="7">
         <v>2</v>
       </c>
       <c r="Q16" s="6" t="s">
@@ -12441,10 +12591,10 @@
       <c r="V16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="X16" s="16" t="s">
+      <c r="X16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="Y16" s="17">
+      <c r="Y16" s="16">
         <v>22.3</v>
       </c>
     </row>
@@ -12462,13 +12612,13 @@
         <v>19</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N18" t="s">
         <v>19</v>
       </c>
       <c r="Q18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="S18" t="s">
         <v>19</v>
@@ -12505,7 +12655,7 @@
       <c r="N19" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="7">
         <v>222068.53551617899</v>
       </c>
       <c r="Q19" s="6" t="s">
@@ -12523,7 +12673,9 @@
       <c r="X19" t="s">
         <v>20</v>
       </c>
-      <c r="Y19" s="7"/>
+      <c r="Y19" s="7">
+        <v>4192.6496664170199</v>
+      </c>
     </row>
     <row r="20" spans="2:25">
       <c r="B20" s="6" t="s">
@@ -12550,7 +12702,7 @@
       <c r="N20" t="s">
         <v>21</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="7">
         <v>471.24148322933002</v>
       </c>
       <c r="Q20" s="6" t="s">
@@ -12568,11 +12720,13 @@
       <c r="X20" t="s">
         <v>21</v>
       </c>
-      <c r="Y20" s="7"/>
+      <c r="Y20" s="7">
+        <v>64.7506730962468</v>
+      </c>
     </row>
     <row r="21" spans="2:25">
       <c r="B21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -12581,7 +12735,7 @@
         <v>31.378240883276199</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
@@ -12590,16 +12744,16 @@
         <v>33.494326075121698</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N21" t="s">
         <v>22</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="7">
         <v>226.05067837524399</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="S21" t="s">
         <v>22</v>
@@ -12608,12 +12762,14 @@
         <v>244.727114253997</v>
       </c>
       <c r="V21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="X21" t="s">
         <v>22</v>
       </c>
-      <c r="Y21" s="7"/>
+      <c r="Y21" s="7">
+        <v>33.545578867809702</v>
+      </c>
     </row>
     <row r="22" spans="2:25">
       <c r="B22" s="6" t="s">
@@ -12640,7 +12796,7 @@
       <c r="N22" t="s">
         <v>23</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22" s="7">
         <v>0.85582288366816905</v>
       </c>
       <c r="Q22" s="6" t="s">
@@ -12658,7 +12814,9 @@
       <c r="X22" t="s">
         <v>23</v>
       </c>
-      <c r="Y22" s="7"/>
+      <c r="Y22" s="7">
+        <v>0.243073881493933</v>
+      </c>
     </row>
     <row r="23" spans="2:25">
       <c r="B23" s="6" t="s">
@@ -12682,19 +12840,19 @@
       <c r="L23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="16" t="s">
+      <c r="N23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O23" s="17">
+      <c r="O23" s="16">
         <v>3.7432172500790499E-2</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S23" s="16" t="s">
+      <c r="S23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T23" s="17">
+      <c r="T23" s="16">
         <v>-8.5260988769203502E-2</v>
       </c>
       <c r="V23" s="6" t="s">
@@ -12703,7 +12861,9 @@
       <c r="X23" t="s">
         <v>24</v>
       </c>
-      <c r="Y23" s="7"/>
+      <c r="Y23" s="7">
+        <v>0.98182673798659603</v>
+      </c>
     </row>
     <row r="24" spans="2:25">
       <c r="B24" s="6" t="s">
@@ -12730,7 +12890,7 @@
       <c r="N24" t="s">
         <v>38</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="7">
         <v>2</v>
       </c>
       <c r="Q24" s="6" t="s">
@@ -12745,10 +12905,12 @@
       <c r="V24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="X24" s="16" t="s">
+      <c r="X24" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="Y24" s="17"/>
+      <c r="Y24" s="16">
+        <v>32.799999999999997</v>
+      </c>
     </row>
     <row r="26" spans="2:25">
       <c r="B26" t="s">
@@ -12764,9 +12926,15 @@
         <v>19</v>
       </c>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N26" t="s">
+        <v>19</v>
+      </c>
+      <c r="V26" t="s">
+        <v>18</v>
+      </c>
+      <c r="X26" t="s">
         <v>19</v>
       </c>
     </row>
@@ -12795,8 +12963,17 @@
       <c r="N27" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="7">
         <v>197521.568445524</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X27" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>4674.3466439106696</v>
       </c>
     </row>
     <row r="28" spans="2:25">
@@ -12824,13 +13001,22 @@
       <c r="N28" t="s">
         <v>21</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28" s="7">
         <v>444.43398660039901</v>
+      </c>
+      <c r="V28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X28" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>68.369193676031202</v>
       </c>
     </row>
     <row r="29" spans="2:25">
       <c r="B29" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -12839,7 +13025,7 @@
         <v>33.435957839053202</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I29" t="s">
         <v>22</v>
@@ -12848,13 +13034,22 @@
         <v>33.669847922623099</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N29" t="s">
         <v>22</v>
       </c>
-      <c r="O29" s="9">
+      <c r="O29" s="7">
         <v>211.689742294311</v>
+      </c>
+      <c r="V29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X29" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>32.186460741875898</v>
       </c>
     </row>
     <row r="30" spans="2:25">
@@ -12882,8 +13077,17 @@
       <c r="N30" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="9">
+      <c r="O30" s="7">
         <v>0.99409821634078999</v>
+      </c>
+      <c r="V30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="X30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>0.21401878211497599</v>
       </c>
     </row>
     <row r="31" spans="2:25">
@@ -12908,11 +13112,20 @@
       <c r="L31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N31" s="16" t="s">
+      <c r="N31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O31" s="17">
+      <c r="O31" s="16">
         <v>0.14383230122669599</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="X31" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y31" s="7">
+        <v>0.97973879692794397</v>
       </c>
     </row>
     <row r="32" spans="2:25">
@@ -12940,11 +13153,20 @@
       <c r="N32" t="s">
         <v>38</v>
       </c>
-      <c r="O32" s="9">
+      <c r="O32" s="7">
         <v>2</v>
       </c>
+      <c r="V32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y32" s="16">
+        <v>22</v>
+      </c>
     </row>
-    <row r="34" spans="2:15">
+    <row r="34" spans="2:25">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -12958,13 +13180,19 @@
         <v>19</v>
       </c>
       <c r="L34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N34" t="s">
         <v>19</v>
       </c>
+      <c r="V34" t="s">
+        <v>18</v>
+      </c>
+      <c r="X34" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:25">
       <c r="B35" s="6" t="s">
         <v>11</v>
       </c>
@@ -12989,11 +13217,18 @@
       <c r="N35" t="s">
         <v>20</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="7">
         <v>176733.441396621</v>
       </c>
+      <c r="V35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X35" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y35" s="7"/>
     </row>
-    <row r="36" spans="2:15">
+    <row r="36" spans="2:25">
       <c r="B36" s="6" t="s">
         <v>12</v>
       </c>
@@ -13018,13 +13253,20 @@
       <c r="N36" t="s">
         <v>21</v>
       </c>
-      <c r="O36" s="9">
+      <c r="O36" s="7">
         <v>420.39676663435603</v>
       </c>
+      <c r="V36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X36" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y36" s="7"/>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="2:25">
       <c r="B37" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -13033,7 +13275,7 @@
         <v>32.316536344024797</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I37" t="s">
         <v>22</v>
@@ -13042,16 +13284,23 @@
         <v>31.930257438063599</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N37" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="9">
+      <c r="O37" s="7">
         <v>202.08229846954299</v>
       </c>
+      <c r="V37" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="X37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y37" s="7"/>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="2:25">
       <c r="B38" s="6" t="s">
         <v>14</v>
       </c>
@@ -13076,11 +13325,18 @@
       <c r="N38" t="s">
         <v>23</v>
       </c>
-      <c r="O38" s="9">
+      <c r="O38" s="7">
         <v>1.17469840524194</v>
       </c>
+      <c r="V38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="X38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y38" s="7"/>
     </row>
-    <row r="39" spans="2:15">
+    <row r="39" spans="2:25">
       <c r="B39" s="6" t="s">
         <v>15</v>
       </c>
@@ -13102,14 +13358,21 @@
       <c r="L39" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N39" s="16" t="s">
+      <c r="N39" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O39" s="17">
+      <c r="O39" s="16">
         <v>0.233939538817687</v>
       </c>
+      <c r="V39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="X39" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y39" s="7"/>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:25">
       <c r="B40" s="6" t="s">
         <v>16</v>
       </c>
@@ -13134,19 +13397,26 @@
       <c r="N40" t="s">
         <v>38</v>
       </c>
-      <c r="O40" s="9">
+      <c r="O40" s="7">
         <v>2.2000000000000002</v>
       </c>
+      <c r="V40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X40" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y40" s="16"/>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:25">
       <c r="G42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:25">
       <c r="G43" s="6" t="s">
         <v>25</v>
       </c>
@@ -13158,7 +13428,7 @@
       </c>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="2:15">
+    <row r="44" spans="2:25">
       <c r="G44" s="6" t="s">
         <v>12</v>
       </c>
@@ -13170,9 +13440,9 @@
       </c>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:25">
       <c r="G45" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I45" t="s">
         <v>22</v>
@@ -13182,7 +13452,7 @@
       </c>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:25">
       <c r="G46" s="6" t="s">
         <v>14</v>
       </c>
@@ -13194,7 +13464,7 @@
       </c>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:25">
       <c r="G47" s="6" t="s">
         <v>15</v>
       </c>
@@ -13206,7 +13476,7 @@
       </c>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:25">
       <c r="G48" s="6" t="s">
         <v>16</v>
       </c>
@@ -13222,7 +13492,7 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="44">
+  <tableParts count="48">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -13267,6 +13537,10 @@
     <tablePart r:id="rId43"/>
     <tablePart r:id="rId44"/>
     <tablePart r:id="rId45"/>
+    <tablePart r:id="rId46"/>
+    <tablePart r:id="rId47"/>
+    <tablePart r:id="rId48"/>
+    <tablePart r:id="rId49"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>